<commit_message>
Genera archivo csv de la web
</commit_message>
<xml_diff>
--- a/dataweb_limpio.xlsx
+++ b/dataweb_limpio.xlsx
@@ -489,13 +489,13 @@
         <v>9419446</v>
       </c>
       <c r="F2" t="n">
-        <v>9662795</v>
+        <v>9658138</v>
       </c>
       <c r="G2" t="n">
-        <v>9662795</v>
+        <v>9658138</v>
       </c>
       <c r="H2" t="n">
-        <v>32949364736</v>
+        <v>33109458944</v>
       </c>
     </row>
     <row r="3">

</xml_diff>